<commit_message>
trigger prob updated from FLEX-Behavior
</commit_message>
<xml_diff>
--- a/tests/behavior/input/BehaviorParam_Technology_TriggerProbability.xlsx
+++ b/tests/behavior/input/BehaviorParam_Technology_TriggerProbability.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX_temp/projects/test_behavior/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/FLEX/tests/behavior/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E28C6C-9835-894A-936E-FE55DB6E2FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0727999E-D54D-F145-95BE-3CC1F35932D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9680" yWindow="-20020" windowWidth="18040" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="5">
   <si>
     <t>value</t>
   </si>
@@ -242,8 +242,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5DEDA1C4-9DD0-5445-B0A4-9BFEFCA653EF}" name="Table1" displayName="Table1" ref="A1:D58" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D58" xr:uid="{5DEDA1C4-9DD0-5445-B0A4-9BFEFCA653EF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5DEDA1C4-9DD0-5445-B0A4-9BFEFCA653EF}" name="Table1" displayName="Table1" ref="A1:D62" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D62" xr:uid="{5DEDA1C4-9DD0-5445-B0A4-9BFEFCA653EF}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D13772B6-3362-0E4E-85D9-C4A4391AA10A}" name="id_activity" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{A6DBB581-D6B6-FE40-937D-2BF0BA88D4B1}" name="id_technology" dataDxfId="2"/>
@@ -551,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -612,88 +612,87 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="4">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F4" s="4"/>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="4">
-        <v>0.11111111111111112</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="4">
-        <v>0.11111111111111112</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>8.8888888888888906E-2</v>
+      </c>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>3</v>
       </c>
       <c r="B7" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="4">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>8.8888888888888906E-2</v>
+      </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
       <c r="B8" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="4">
-        <v>0.11111111111111112</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="4">
-        <v>0.29659259259259263</v>
+        <v>8.8888888888888906E-2</v>
       </c>
       <c r="F9" s="4"/>
     </row>
@@ -702,298 +701,298 @@
         <v>4</v>
       </c>
       <c r="B10" s="2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="4">
-        <v>0.17056790123456775</v>
-      </c>
-      <c r="F10" s="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>4</v>
       </c>
       <c r="B11" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="4">
-        <v>0.2494814814814815</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>0.26693333333333336</v>
+      </c>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>4</v>
       </c>
       <c r="B12" s="2">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="4">
-        <v>3.6641975308641973E-2</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>0.15351111111111099</v>
+      </c>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>4</v>
       </c>
       <c r="B13" s="2">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="4">
-        <v>3.2691358024691357E-2</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>0.22453333333333336</v>
+      </c>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>4</v>
       </c>
       <c r="B14" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="4">
-        <v>5.4716049382716049E-2</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>3.2977777777777779E-2</v>
+      </c>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>4</v>
       </c>
       <c r="B15" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="4">
-        <v>3.5654320987654323E-2</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>2.9422222222222221E-2</v>
+      </c>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>4</v>
       </c>
       <c r="B16" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="4">
-        <v>5.649382716049383E-2</v>
-      </c>
-      <c r="F16" s="2"/>
+        <v>4.9244444444444445E-2</v>
+      </c>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
       <c r="B17" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="4">
-        <v>6.7160493827160495E-2</v>
-      </c>
-      <c r="F17" s="2"/>
+        <v>3.2088888888888889E-2</v>
+      </c>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="F18" s="2"/>
+        <v>5.0844444444444449E-2</v>
+      </c>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="F19" s="2"/>
+        <v>6.0444444444444446E-2</v>
+      </c>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F20" s="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="4">
-        <v>0.7</v>
+        <v>0.32000000000000006</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="4">
-        <v>1</v>
+        <v>0.48</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B23" s="2">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="4">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24" s="2">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="4">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B25" s="2">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="4">
-        <v>0.21361820199778001</v>
+        <v>0.55999999999999994</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B26" s="2">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="4">
-        <v>0.124461709211987</v>
+        <v>1</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" s="2">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="4">
-        <v>9.0665926748057679E-2</v>
+        <v>0.8</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" s="2">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="4">
-        <v>0.16167591564927855</v>
+        <v>0.2</v>
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>9</v>
       </c>
       <c r="B29" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="4">
-        <v>3.1620421753607089E-2</v>
+        <v>0.21361820199778001</v>
       </c>
       <c r="F29" s="2"/>
     </row>
@@ -1002,13 +1001,13 @@
         <v>9</v>
       </c>
       <c r="B30" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="4">
-        <v>0.159034406215316</v>
+        <v>0.124461709211987</v>
       </c>
       <c r="F30" s="2"/>
     </row>
@@ -1017,13 +1016,13 @@
         <v>9</v>
       </c>
       <c r="B31" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="4">
-        <v>6.3573806881243047E-2</v>
+        <v>9.0665926748057679E-2</v>
       </c>
       <c r="F31" s="2"/>
     </row>
@@ -1032,13 +1031,13 @@
         <v>9</v>
       </c>
       <c r="B32" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D32" s="4">
-        <v>0.145528301886792</v>
+        <v>0.16167591564927855</v>
       </c>
       <c r="F32" s="2"/>
     </row>
@@ -1047,91 +1046,88 @@
         <v>9</v>
       </c>
       <c r="B33" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="4">
-        <v>9.7114317425083235E-3</v>
+        <v>3.1620421753607089E-2</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>10</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B34" s="2">
+        <v>7</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="6">
-        <v>1</v>
+      <c r="D34" s="4">
+        <v>0.159034406215316</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>11</v>
-      </c>
-      <c r="B35" s="3">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B35" s="2">
+        <v>8</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="5"/>
+      <c r="D35" s="4">
+        <v>6.3573806881243047E-2</v>
+      </c>
+      <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B36" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="4">
-        <v>0.41111111111111098</v>
-      </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="5"/>
+        <v>0.145528301886792</v>
+      </c>
+      <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B37" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="4">
-        <v>0.24444444444444399</v>
+        <v>9.7114317425083235E-3</v>
       </c>
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>11</v>
-      </c>
-      <c r="B38" s="2">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="4">
-        <v>5.5555555555555559E-2</v>
+      <c r="D38" s="6">
+        <v>1</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -1139,90 +1135,92 @@
       <c r="A39" s="2">
         <v>11</v>
       </c>
-      <c r="B39" s="2">
-        <v>5</v>
+      <c r="B39" s="3">
+        <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="4">
-        <v>0.11111111111111112</v>
-      </c>
-      <c r="F39" s="2"/>
+      <c r="D39" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>11</v>
       </c>
       <c r="B40" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="4">
-        <v>7.7777777777777779E-2</v>
-      </c>
-      <c r="F40" s="2"/>
+        <v>0.41111111111111098</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>12</v>
-      </c>
-      <c r="B41" s="3">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="B41" s="2">
+        <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="F41" s="4"/>
-      <c r="G41" s="5"/>
+      <c r="D41" s="4">
+        <v>0.24444444444444399</v>
+      </c>
+      <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D42" s="4">
-        <v>0.24444444444444399</v>
+        <v>5.5555555555555559E-2</v>
       </c>
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D43" s="4">
-        <v>0.41111111111111109</v>
+        <v>0.11111111111111112</v>
       </c>
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D44" s="4">
-        <v>5.5555555555555559E-2</v>
+        <v>7.7777777777777779E-2</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -1230,227 +1228,276 @@
       <c r="A45" s="2">
         <v>12</v>
       </c>
-      <c r="B45" s="2">
-        <v>5</v>
+      <c r="B45" s="3">
+        <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="4">
-        <v>0.11111111111111112</v>
-      </c>
-      <c r="F45" s="2"/>
+      <c r="D45" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="F45" s="4"/>
+      <c r="G45" s="5"/>
     </row>
     <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>12</v>
       </c>
       <c r="B46" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="4">
-        <v>7.7777777777777779E-2</v>
+        <v>0.24444444444444399</v>
       </c>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>13</v>
-      </c>
-      <c r="B47" s="3">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B47" s="2">
+        <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D47" s="6">
-        <v>1</v>
+      <c r="D47" s="4">
+        <v>0.41111111111111109</v>
       </c>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>14</v>
-      </c>
-      <c r="B48" s="3">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B48" s="2">
+        <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D48" s="6">
-        <v>1</v>
+      <c r="D48" s="4">
+        <v>5.5555555555555559E-2</v>
       </c>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>15</v>
-      </c>
-      <c r="B49" s="3">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B49" s="2">
+        <v>5</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D49" s="6">
-        <v>1</v>
+      <c r="D49" s="4">
+        <v>0.11111111111111112</v>
       </c>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B50" s="2">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D50" s="4">
-        <v>0.46241872444730298</v>
-      </c>
-      <c r="F50" s="4"/>
-      <c r="G50" s="5"/>
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>16</v>
-      </c>
-      <c r="B51" s="2">
-        <v>33</v>
+        <v>13</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="4">
-        <v>0.34690222387026898</v>
+      <c r="D51" s="6">
+        <v>1</v>
       </c>
       <c r="F51" s="2"/>
-      <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>16</v>
-      </c>
-      <c r="B52" s="2">
-        <v>34</v>
+        <v>14</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D52" s="4">
-        <v>0.19067905168242799</v>
+      <c r="D52" s="6">
+        <v>1</v>
       </c>
       <c r="F52" s="2"/>
-      <c r="G52" s="5"/>
     </row>
     <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>17</v>
-      </c>
-      <c r="B53" s="2">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="4">
-        <v>0.41666666666666657</v>
-      </c>
-      <c r="F53" s="4"/>
-      <c r="G53" s="5"/>
+      <c r="D53" s="6">
+        <v>1</v>
+      </c>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B54" s="2">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="4">
-        <v>0.1148680273473412</v>
-      </c>
-      <c r="F54" s="2"/>
+        <v>0.46241872444730298</v>
+      </c>
+      <c r="F54" s="4"/>
+      <c r="G54" s="5"/>
     </row>
     <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B55" s="2">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D55" s="4">
-        <v>7.8481520485432013E-2</v>
+        <v>0.34690222387026898</v>
       </c>
       <c r="F55" s="2"/>
+      <c r="G55" s="5"/>
     </row>
     <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B56" s="2">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D56" s="4">
-        <v>7.8397940591411308E-2</v>
+        <v>0.19067905168242799</v>
       </c>
       <c r="F56" s="2"/>
+      <c r="G56" s="5"/>
     </row>
     <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>17</v>
       </c>
       <c r="B57" s="2">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D57" s="4">
-        <v>0.14166792036507697</v>
-      </c>
-      <c r="F57" s="2"/>
+        <v>0.41666666666666657</v>
+      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="5"/>
     </row>
     <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>17</v>
       </c>
       <c r="B58" s="2">
+        <v>14</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0.1148680273473412</v>
+      </c>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>17</v>
+      </c>
+      <c r="B59" s="2">
+        <v>17</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="4">
+        <v>7.8481520485432013E-2</v>
+      </c>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>17</v>
+      </c>
+      <c r="B60" s="2">
+        <v>18</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" s="4">
+        <v>7.8397940591411308E-2</v>
+      </c>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>17</v>
+      </c>
+      <c r="B61" s="2">
+        <v>20</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="4">
+        <v>0.14166792036507697</v>
+      </c>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>17</v>
+      </c>
+      <c r="B62" s="2">
         <v>21</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58" s="4">
+      <c r="C62" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" s="4">
         <v>0.16991792454407165</v>
       </c>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F59" s="7"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F60" s="7"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F61" s="7"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F62" s="7"/>
+      <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F63" s="7"/>
@@ -1481,6 +1528,18 @@
     </row>
     <row r="72" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F73" s="7"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F74" s="7"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F75" s="7"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F76" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1491,6 +1550,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001383FD7952F44C4AA66F138C1496F932" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4511c60809de47fd61668c7a2fa421c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ed526690-1b82-4476-9598-c0eeafad58f9" xmlns:ns3="f971c2dd-4979-4752-97a1-eb062e2c22bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="113b7667aea05225525c2a1f4252ac59" ns2:_="" ns3:_="">
     <xsd:import namespace="ed526690-1b82-4476-9598-c0eeafad58f9"/>
@@ -1695,15 +1763,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1716,6 +1775,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD38B489-F981-428C-BF72-292671E2847C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D125F7-70BC-4CD8-BA77-1F77C7034327}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1734,14 +1801,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD38B489-F981-428C-BF72-292671E2847C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E8BF163-7E87-4B8A-965E-CB930C72B92B}">
   <ds:schemaRefs>

</xml_diff>